<commit_message>
Verschiebung der Stunde am 12.03.2015 eingetragen
</commit_message>
<xml_diff>
--- a/nvs_Zojer_Projekt.xlsx
+++ b/nvs_Zojer_Projekt.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstanze\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\NVS-ZH\Konzepte\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +204,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -225,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -238,6 +252,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -256,9 +273,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -296,7 +313,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -368,7 +385,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -518,228 +535,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>42019</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>42026</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
+      <c r="D3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>42033</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>42040</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>42047</v>
       </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>42054</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>42061</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>42068</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>42075</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>42082</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>42089</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>42096</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>42054</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>42103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>42061</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>42110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
-        <v>42068</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>42117</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <v>42075</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>42082</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
-        <v>42089</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <v>42096</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <v>42103</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>42110</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
-        <v>42117</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>42124</v>
       </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
       <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="s">
         <v>19</v>
       </c>
-      <c r="E17">
+      <c r="D17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>42131</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>1</v>
       </c>
+      <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
-        <f>COUNT(B2:B17)*2</f>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <f>COUNT(A2:A17)*2</f>
         <v>32</v>
       </c>
-      <c r="E20">
-        <f>SUM(E2:E19)</f>
-        <v>30</v>
+      <c r="D20">
+        <f>SUM(D2:D19)</f>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -752,36 +773,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -798,7 +820,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -815,7 +837,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -832,7 +854,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -849,7 +871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -866,7 +888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -885,5 +907,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>